<commit_message>
// adding houses but keep streets clear
</commit_message>
<xml_diff>
--- a/auxfiles/cukvertN.xlsx
+++ b/auxfiles/cukvertN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prgc\lisemgit\openlisem\auxfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C425FB38-F0A3-4803-B85D-FD8CD881CB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC673C0-02D7-478F-8F60-B5CF65B3C41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{E7372BA5-4E66-4B5A-980A-99B2857E7BC6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>h</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>R2/3</t>
+  </si>
+  <si>
+    <t>n*(0.1+Q/qmax)</t>
   </si>
 </sst>
 </file>
@@ -1697,12 +1700,13 @@
   <dimension ref="C3:M43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:13" x14ac:dyDescent="0.3">
@@ -1740,6 +1744,9 @@
       <c r="J5" t="s">
         <v>5</v>
       </c>
+      <c r="K5" t="s">
+        <v>8</v>
+      </c>
       <c r="L5" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
// mass balances problems!
</commit_message>
<xml_diff>
--- a/auxfiles/cukvertN.xlsx
+++ b/auxfiles/cukvertN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prgc\lisemgit\openlisem\auxfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC673C0-02D7-478F-8F60-B5CF65B3C41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1068727F-8105-4BCC-BBCB-2B9FE0EE2FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{E7372BA5-4E66-4B5A-980A-99B2857E7BC6}"/>
   </bookViews>
@@ -189,118 +189,118 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -334,118 +334,118 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>6.7045123548135882E-2</c:v>
+                  <c:v>7.7427380074318139E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13363785151897248</c:v>
+                  <c:v>0.18238490530892423</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17257395394102465</c:v>
+                  <c:v>0.26353119432340594</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19512195121951226</c:v>
+                  <c:v>0.32000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20898019490925357</c:v>
+                  <c:v>0.35904806348847795</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.21803576282752282</c:v>
+                  <c:v>0.38663726473607829</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.22426922523132259</c:v>
+                  <c:v>0.4066815273330876</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.22874697646296596</c:v>
+                  <c:v>0.42164871285155531</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.23207769344039994</c:v>
+                  <c:v>0.43310632925738418</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.23462754689102505</c:v>
+                  <c:v>0.44207215960481672</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2366270715627154</c:v>
+                  <c:v>0.4492243621368664</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.23822718347183378</c:v>
+                  <c:v>0.45502658876385088</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.23953004568741337</c:v>
+                  <c:v>0.45980360061021947</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.24060685007554777</c:v>
+                  <c:v>0.46378798003267263</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.24150847186789817</c:v>
+                  <c:v>0.46714968496854481</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.24227207862538794</c:v>
+                  <c:v>0.47001519535254632</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.24292535705534848</c:v>
+                  <c:v>0.47248019927747331</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.24348929065284616</c:v>
+                  <c:v>0.47461817729277561</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.24398002969698987</c:v>
+                  <c:v>0.47648632528202672</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.24441017775593737</c:v>
+                  <c:v>0.47812971504504997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.24478969418698746</c:v>
+                  <c:v>0.47958426562589512</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.24512653850750499</c:v>
+                  <c:v>0.48087889785010607</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.24542713788578183</c:v>
+                  <c:v>0.48203711866127152</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.24569673128863817</c:v>
+                  <c:v>0.48307820134138307</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.24593962623279486</c:v>
+                  <c:v>0.48401807528266633</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.24615939269636478</c:v>
+                  <c:v>0.48487000427381877</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.24635901123354623</c:v>
+                  <c:v>0.48564510892280766</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.24654098729521007</c:v>
+                  <c:v>0.48635277290841999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.24670744032332501</c:v>
+                  <c:v>0.48700096173026974</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.24686017381241926</c:v>
+                  <c:v>0.48759647490136904</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.24700073086716265</c:v>
+                  <c:v>0.48814514704679801</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.24713043860431708</c:v>
+                  <c:v>0.48865200943978887</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.2472504438995565</c:v>
+                  <c:v>0.48912142065503456</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.2473617423643458</c:v>
+                  <c:v>0.48955717293039985</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.24746520198687216</c:v>
+                  <c:v>0.48996257928384174</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.24756158253697361</c:v>
+                  <c:v>0.49034054528018289</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.24765155158543958</c:v>
+                  <c:v>0.4906936284755658</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.24773569780001886</c:v>
+                  <c:v>0.49102408791004387</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -599,6 +599,151 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-8B10-4712-8B49-DDCBF9BD646A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$6:$N$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>9.1614288791279658E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8711624283209614E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.57221899881001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.8888888888888906E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12736542412069948</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17053102319555966</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.21789979824502809</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26907580474887255</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.32372743523361935</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.38157141418444396</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.44236210616177418</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.45502658876385088</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.45980360061021947</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.46378798003267263</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.46714968496854481</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.47001519535254632</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.47248019927747331</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.47461817729277561</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.47648632528202672</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.47812971504504997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.47958426562589512</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.48087889785010607</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.48203711866127152</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.48307820134138307</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.48401807528266633</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.48487000427381877</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.48564510892280766</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.48635277290841999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.48700096173026974</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.48759647490136904</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.48814514704679801</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.48865200943978887</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.48912142065503456</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.48955717293039985</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.48996257928384174</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.49034054528018289</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.4906936284755658</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.49102408791004387</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-278B-4E11-995B-DD5CE8EF9A3F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1365,12 +1510,12 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
@@ -1697,10 +1842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCF5D42-AFF0-4820-B50F-3BBD607733D8}">
-  <dimension ref="C3:M43"/>
+  <dimension ref="C3:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="N43" sqref="N6:N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1709,17 +1854,17 @@
     <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.3">
       <c r="H3">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.3">
       <c r="H4">
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -1751,7 +1896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>0.01</v>
       </c>
@@ -1779,22 +1924,26 @@
         <v>9.1614288791279658E-3</v>
       </c>
       <c r="J6">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="K6">
         <f>($H$3+I6/J6)*$H$5</f>
-        <v>6.8322857758255928E-4</v>
+        <v>5.916142887912797E-4</v>
       </c>
       <c r="L6">
         <f>G6*SQRT($H$4)/K6</f>
-        <v>6.7045123548135885</v>
+        <v>7.7427380074318144</v>
       </c>
       <c r="M6">
         <f>L6*E6</f>
-        <v>6.7045123548135882E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
+        <v>7.7427380074318139E-2</v>
+      </c>
+      <c r="N6">
+        <f>MIN(M6,I6)</f>
+        <v>9.1614288791279658E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>0.02</v>
       </c>
@@ -1824,27 +1973,31 @@
       </c>
       <c r="J7">
         <f>J6</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="K7">
         <f t="shared" ref="K7:K43" si="5">($H$3+I7/J7)*$H$5</f>
-        <v>1.0742324856641923E-3</v>
+        <v>7.8711624283209615E-4</v>
       </c>
       <c r="L7">
         <f t="shared" ref="L7:L27" si="6">G7*SQRT($H$4)/K7</f>
-        <v>6.6818925759486243</v>
+        <v>9.1192452654462119</v>
       </c>
       <c r="M7">
         <f t="shared" ref="M7:M27" si="7">L7*E7</f>
-        <v>0.13363785151897248</v>
-      </c>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.18238490530892423</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ref="N7:N43" si="8">MIN(M7,I7)</f>
+        <v>2.8711624283209614E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>0.03</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D43" si="8">D7</f>
+        <f t="shared" ref="D8:D43" si="9">D7</f>
         <v>1</v>
       </c>
       <c r="E8">
@@ -1868,28 +2021,32 @@
         <v>5.57221899881001E-2</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:J43" si="9">J7</f>
-        <v>0.25</v>
+        <f t="shared" ref="J8:J43" si="10">J7</f>
+        <v>0.5</v>
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
-        <v>1.614443799762002E-3</v>
+        <v>1.057221899881001E-3</v>
       </c>
       <c r="L8">
         <f t="shared" si="6"/>
-        <v>5.7524651313674884</v>
+        <v>8.7843731441135322</v>
       </c>
       <c r="M8">
         <f t="shared" si="7"/>
-        <v>0.17257395394102465</v>
-      </c>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.26353119432340594</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="8"/>
+        <v>5.57221899881001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>0.04</v>
       </c>
       <c r="D9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E9">
@@ -1913,28 +2070,32 @@
         <v>8.8888888888888906E-2</v>
       </c>
       <c r="J9">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>2.2777777777777779E-3</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="L9">
         <f t="shared" si="6"/>
-        <v>4.8780487804878065</v>
+        <v>8.0000000000000018</v>
       </c>
       <c r="M9">
         <f t="shared" si="7"/>
-        <v>0.19512195121951226</v>
-      </c>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.32000000000000006</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="8"/>
+        <v>8.8888888888888906E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>0.05</v>
       </c>
       <c r="D10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E10">
@@ -1958,28 +2119,32 @@
         <v>0.12736542412069948</v>
       </c>
       <c r="J10">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K10">
         <f t="shared" si="5"/>
-        <v>3.0473084824139897E-3</v>
+        <v>1.7736542412069951E-3</v>
       </c>
       <c r="L10">
         <f t="shared" si="6"/>
-        <v>4.1796038981850714</v>
+        <v>7.1809612697695586</v>
       </c>
       <c r="M10">
         <f t="shared" si="7"/>
-        <v>0.20898019490925357</v>
-      </c>
-    </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.35904806348847795</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="8"/>
+        <v>0.12736542412069948</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>0.06</v>
       </c>
       <c r="D11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E11">
@@ -2003,28 +2168,32 @@
         <v>0.17053102319555966</v>
       </c>
       <c r="J11">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K11">
         <f t="shared" si="5"/>
-        <v>3.9106204639111934E-3</v>
+        <v>2.2053102319555969E-3</v>
       </c>
       <c r="L11">
         <f t="shared" si="6"/>
-        <v>3.6339293804587141</v>
+        <v>6.4439544122679715</v>
       </c>
       <c r="M11">
         <f t="shared" si="7"/>
-        <v>0.21803576282752282</v>
-      </c>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.38663726473607829</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="8"/>
+        <v>0.17053102319555966</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E12">
@@ -2048,28 +2217,32 @@
         <v>0.21789979824502809</v>
       </c>
       <c r="J12">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K12">
         <f t="shared" si="5"/>
-        <v>4.8579959649005617E-3</v>
+        <v>2.6789979824502807E-3</v>
       </c>
       <c r="L12">
         <f t="shared" si="6"/>
-        <v>3.2038460747331796</v>
+        <v>5.809736104758394</v>
       </c>
       <c r="M12">
         <f t="shared" si="7"/>
-        <v>0.22426922523132259</v>
-      </c>
-    </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.4066815273330876</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="8"/>
+        <v>0.21789979824502809</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>0.08</v>
       </c>
       <c r="D13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E13">
@@ -2093,28 +2266,32 @@
         <v>0.26907580474887255</v>
       </c>
       <c r="J13">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>5.8815160949774519E-3</v>
+        <v>3.1907580474887253E-3</v>
       </c>
       <c r="L13">
         <f t="shared" si="6"/>
-        <v>2.8593372057870745</v>
+        <v>5.2706089106444409</v>
       </c>
       <c r="M13">
         <f t="shared" si="7"/>
-        <v>0.22874697646296596</v>
-      </c>
-    </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.42164871285155531</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="8"/>
+        <v>0.26907580474887255</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>0.09</v>
       </c>
       <c r="D14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E14">
@@ -2138,28 +2315,32 @@
         <v>0.32372743523361935</v>
       </c>
       <c r="J14">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K14">
         <f t="shared" si="5"/>
-        <v>6.9745487046723878E-3</v>
+        <v>3.7372743523361937E-3</v>
       </c>
       <c r="L14">
         <f t="shared" si="6"/>
-        <v>2.578641038226666</v>
+        <v>4.8122925473042688</v>
       </c>
       <c r="M14">
         <f t="shared" si="7"/>
-        <v>0.23207769344039994</v>
-      </c>
-    </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.43310632925738418</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="8"/>
+        <v>0.32372743523361935</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>0.1</v>
       </c>
       <c r="D15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E15">
@@ -2183,28 +2364,32 @@
         <v>0.38157141418444396</v>
       </c>
       <c r="J15">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K15">
         <f t="shared" si="5"/>
-        <v>8.1314282836888793E-3</v>
+        <v>4.3157141418444398E-3</v>
       </c>
       <c r="L15">
         <f t="shared" si="6"/>
-        <v>2.3462754689102505</v>
+        <v>4.4207215960481667</v>
       </c>
       <c r="M15">
         <f t="shared" si="7"/>
-        <v>0.23462754689102505</v>
-      </c>
-    </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.44207215960481672</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="8"/>
+        <v>0.38157141418444396</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>0.11</v>
       </c>
       <c r="D16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E16">
@@ -2228,28 +2413,32 @@
         <v>0.44236210616177418</v>
       </c>
       <c r="J16">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K16">
         <f t="shared" si="5"/>
-        <v>9.3472421232354847E-3</v>
+        <v>4.9236210616177417E-3</v>
       </c>
       <c r="L16">
         <f t="shared" si="6"/>
-        <v>2.1511551960246855</v>
+        <v>4.0838578376078765</v>
       </c>
       <c r="M16">
         <f t="shared" si="7"/>
-        <v>0.2366270715627154</v>
-      </c>
-    </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.4492243621368664</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="8"/>
+        <v>0.44236210616177418</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>0.12</v>
       </c>
       <c r="D17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E17">
@@ -2273,28 +2462,32 @@
         <v>0.50588400596807026</v>
       </c>
       <c r="J17">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K17">
         <f t="shared" si="5"/>
-        <v>1.0617680119361405E-2</v>
+        <v>5.5588400596807029E-3</v>
       </c>
       <c r="L17">
         <f t="shared" si="6"/>
-        <v>1.9852265289319482</v>
+        <v>3.7918882396987574</v>
       </c>
       <c r="M17">
         <f t="shared" si="7"/>
-        <v>0.23822718347183378</v>
-      </c>
-    </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.45502658876385088</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="8"/>
+        <v>0.45502658876385088</v>
+      </c>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>0.13</v>
       </c>
       <c r="D18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E18">
@@ -2318,28 +2511,32 @@
         <v>0.57194625338397864</v>
       </c>
       <c r="J18">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K18">
         <f t="shared" si="5"/>
-        <v>1.1938925067679573E-2</v>
+        <v>6.2194625338397869E-3</v>
       </c>
       <c r="L18">
         <f t="shared" si="6"/>
-        <v>1.8425388129801028</v>
+        <v>3.5369507739247652</v>
       </c>
       <c r="M18">
         <f t="shared" si="7"/>
-        <v>0.23953004568741337</v>
-      </c>
-    </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.45980360061021947</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="8"/>
+        <v>0.45980360061021947</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>0.14000000000000001</v>
       </c>
       <c r="D19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E19">
@@ -2363,28 +2560,32 @@
         <v>0.64037849925402024</v>
       </c>
       <c r="J19">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K19">
         <f t="shared" si="5"/>
-        <v>1.3307569985080406E-2</v>
+        <v>6.9037849925402033E-3</v>
       </c>
       <c r="L19">
         <f t="shared" si="6"/>
-        <v>1.7186203576824839</v>
+        <v>3.3127712859476612</v>
       </c>
       <c r="M19">
         <f t="shared" si="7"/>
-        <v>0.24060685007554777</v>
-      </c>
-    </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.46378798003267263</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="8"/>
+        <v>0.46378798003267263</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>0.15</v>
       </c>
       <c r="D20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E20">
@@ -2408,28 +2609,32 @@
         <v>0.71102770935565829</v>
       </c>
       <c r="J20">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K20">
         <f t="shared" si="5"/>
-        <v>1.4720554187113167E-2</v>
+        <v>7.6102770935565838E-3</v>
       </c>
       <c r="L20">
         <f t="shared" si="6"/>
-        <v>1.6100564791193213</v>
+        <v>3.1143312331236324</v>
       </c>
       <c r="M20">
         <f t="shared" si="7"/>
-        <v>0.24150847186789817</v>
-      </c>
-    </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.46714968496854481</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="8"/>
+        <v>0.46714968496854481</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>0.16</v>
       </c>
       <c r="D21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E21">
@@ -2453,28 +2658,32 @@
         <v>0.78375564036309164</v>
       </c>
       <c r="J21">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K21">
         <f t="shared" si="5"/>
-        <v>1.6175112807261832E-2</v>
+        <v>8.3375564036309163E-3</v>
       </c>
       <c r="L21">
         <f t="shared" si="6"/>
-        <v>1.5142004914086746</v>
+        <v>2.9375949709534144</v>
       </c>
       <c r="M21">
         <f t="shared" si="7"/>
-        <v>0.24227207862538794</v>
-      </c>
-    </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.47001519535254632</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="8"/>
+        <v>0.47001519535254632</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>0.17</v>
       </c>
       <c r="D22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E22">
@@ -2498,28 +2707,32 @@
         <v>0.85843681071919919</v>
       </c>
       <c r="J22">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K22">
         <f t="shared" si="5"/>
-        <v>1.7668736214383984E-2</v>
+        <v>9.084368107191992E-3</v>
       </c>
       <c r="L22">
         <f t="shared" si="6"/>
-        <v>1.4289726885608733</v>
+        <v>2.7792952898674899</v>
       </c>
       <c r="M22">
         <f t="shared" si="7"/>
-        <v>0.24292535705534848</v>
-      </c>
-    </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.47248019927747331</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="8"/>
+        <v>0.47248019927747331</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>0.18</v>
       </c>
       <c r="D23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E23">
@@ -2543,28 +2756,32 @@
         <v>0.93495684444617699</v>
       </c>
       <c r="J23">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K23">
         <f t="shared" si="5"/>
-        <v>1.9199136888923541E-2</v>
+        <v>9.8495684444617707E-3</v>
       </c>
       <c r="L23">
         <f t="shared" si="6"/>
-        <v>1.352718281404701</v>
+        <v>2.6367676516265313</v>
       </c>
       <c r="M23">
         <f t="shared" si="7"/>
-        <v>0.24348929065284616</v>
-      </c>
-    </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.47461817729277561</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="8"/>
+        <v>0.47461817729277561</v>
+      </c>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>0.19</v>
       </c>
       <c r="D24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E24">
@@ -2588,28 +2805,32 @@
         <v>1.0132111016186967</v>
       </c>
       <c r="J24">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K24">
         <f t="shared" si="5"/>
-        <v>2.0764222032373932E-2</v>
+        <v>1.0632111016186966E-2</v>
       </c>
       <c r="L24">
         <f t="shared" si="6"/>
-        <v>1.2841054194578414</v>
+        <v>2.507822764642246</v>
       </c>
       <c r="M24">
         <f t="shared" si="7"/>
-        <v>0.24398002969698987</v>
-      </c>
-    </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.47648632528202672</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="8"/>
+        <v>0.47648632528202672</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>0.2</v>
       </c>
       <c r="D25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E25">
@@ -2633,28 +2854,32 @@
         <v>1.0931035330127941</v>
       </c>
       <c r="J25">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K25">
         <f t="shared" si="5"/>
-        <v>2.2362070660255879E-2</v>
+        <v>1.1431035330127941E-2</v>
       </c>
       <c r="L25">
         <f t="shared" si="6"/>
-        <v>1.2220508887796868</v>
+        <v>2.3906485752252498</v>
       </c>
       <c r="M25">
         <f t="shared" si="7"/>
-        <v>0.24441017775593737</v>
-      </c>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.47812971504504997</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="8"/>
+        <v>0.47812971504504997</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>0.21</v>
       </c>
       <c r="D26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E26">
@@ -2678,28 +2903,32 @@
         <v>1.1745457127278149</v>
       </c>
       <c r="J26">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K26">
         <f t="shared" si="5"/>
-        <v>2.3990914254556298E-2</v>
+        <v>1.2245457127278149E-2</v>
       </c>
       <c r="L26">
         <f t="shared" si="6"/>
-        <v>1.165665210414226</v>
+        <v>2.2837345982185484</v>
       </c>
       <c r="M26">
         <f t="shared" si="7"/>
-        <v>0.24478969418698746</v>
-      </c>
-    </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.47958426562589512</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="8"/>
+        <v>0.47958426562589512</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>0.22</v>
       </c>
       <c r="D27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E27">
@@ -2723,40 +2952,44 @@
         <v>1.2574560139902171</v>
       </c>
       <c r="J27">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K27">
         <f t="shared" si="5"/>
-        <v>2.564912027980434E-2</v>
+        <v>1.3074560139902172E-2</v>
       </c>
       <c r="L27">
         <f t="shared" si="6"/>
-        <v>1.1142115386704772</v>
+        <v>2.1858131720459366</v>
       </c>
       <c r="M27">
         <f t="shared" si="7"/>
-        <v>0.24512653850750499</v>
-      </c>
-    </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.3">
+        <v>0.48087889785010607</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="8"/>
+        <v>0.48087889785010607</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>0.23</v>
       </c>
       <c r="D28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E28">
-        <f t="shared" ref="E28:E43" si="10">D28*C28</f>
+        <f t="shared" ref="E28:E43" si="11">D28*C28</f>
         <v>0.23</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F28:F43" si="11">D28+2*C28</f>
+        <f t="shared" ref="F28:F43" si="12">D28+2*C28</f>
         <v>1.46</v>
       </c>
       <c r="G28">
-        <f t="shared" ref="G28:G43" si="12">(E28/F28)^(2/3)</f>
+        <f t="shared" ref="G28:G43" si="13">(E28/F28)^(2/3)</f>
         <v>0.29168671772025279</v>
       </c>
       <c r="H28">
@@ -2764,44 +2997,48 @@
         <v>5.8337343544050562</v>
       </c>
       <c r="I28">
-        <f t="shared" ref="I28:I43" si="13">H28*E28</f>
+        <f t="shared" ref="I28:I43" si="14">H28*E28</f>
         <v>1.341758901513163</v>
       </c>
       <c r="J28">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K28">
         <f t="shared" si="5"/>
-        <v>2.7335178030263259E-2</v>
+        <v>1.3917589015131631E-2</v>
       </c>
       <c r="L28">
-        <f t="shared" ref="L28:L43" si="14">G28*SQRT($H$4)/K28</f>
-        <v>1.0670745125468775</v>
+        <f t="shared" ref="L28:L43" si="15">G28*SQRT($H$4)/K28</f>
+        <v>2.0958135593968326</v>
       </c>
       <c r="M28">
-        <f t="shared" ref="M28:M43" si="15">L28*E28</f>
-        <v>0.24542713788578183</v>
-      </c>
-    </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" ref="M28:M43" si="16">L28*E28</f>
+        <v>0.48203711866127152</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="8"/>
+        <v>0.48203711866127152</v>
+      </c>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>0.24</v>
       </c>
       <c r="D29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.24</v>
       </c>
       <c r="F29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.48</v>
       </c>
       <c r="G29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.29737173327869948</v>
       </c>
       <c r="H29">
@@ -2809,44 +3046,48 @@
         <v>5.94743466557399</v>
       </c>
       <c r="I29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.4273843197377576</v>
       </c>
       <c r="J29">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K29">
         <f t="shared" si="5"/>
-        <v>2.9047686394755152E-2</v>
+        <v>1.4773843197377576E-2</v>
       </c>
       <c r="L29">
-        <f t="shared" si="14"/>
-        <v>1.0237363803693258</v>
+        <f t="shared" si="15"/>
+        <v>2.0128258389224296</v>
       </c>
       <c r="M29">
-        <f t="shared" si="15"/>
-        <v>0.24569673128863817</v>
-      </c>
-    </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.48307820134138307</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="8"/>
+        <v>0.48307820134138307</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>0.25</v>
       </c>
       <c r="D30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.5</v>
       </c>
       <c r="G30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.30285343213868998</v>
       </c>
       <c r="H30">
@@ -2854,44 +3095,48 @@
         <v>6.0570686427737996</v>
       </c>
       <c r="I30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.5142671606934499</v>
       </c>
       <c r="J30">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K30">
         <f t="shared" si="5"/>
-        <v>3.0785343213868999E-2</v>
+        <v>1.56426716069345E-2</v>
       </c>
       <c r="L30">
-        <f t="shared" si="14"/>
-        <v>0.98375850493117944</v>
+        <f t="shared" si="15"/>
+        <v>1.9360723011306653</v>
       </c>
       <c r="M30">
-        <f t="shared" si="15"/>
-        <v>0.24593962623279486</v>
-      </c>
-    </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.48401807528266633</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="8"/>
+        <v>0.48401807528266633</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>0.26</v>
       </c>
       <c r="D31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.26</v>
       </c>
       <c r="F31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.52</v>
       </c>
       <c r="G31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.3081436151028345</v>
       </c>
       <c r="H31">
@@ -2899,44 +3144,48 @@
         <v>6.16287230205669</v>
       </c>
       <c r="I31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.6023467985347395</v>
       </c>
       <c r="J31">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K31">
         <f t="shared" si="5"/>
-        <v>3.2546935970694787E-2</v>
+        <v>1.6523467985347394E-2</v>
       </c>
       <c r="L31">
-        <f t="shared" si="14"/>
-        <v>0.94676689498601829</v>
+        <f t="shared" si="15"/>
+        <v>1.8648846318223797</v>
       </c>
       <c r="M31">
-        <f t="shared" si="15"/>
-        <v>0.24615939269636478</v>
-      </c>
-    </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.48487000427381877</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="8"/>
+        <v>0.48487000427381877</v>
+      </c>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C32">
         <v>0.27</v>
       </c>
       <c r="D32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.27</v>
       </c>
       <c r="F32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.54</v>
       </c>
       <c r="G32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.31325308895252124</v>
       </c>
       <c r="H32">
@@ -2944,44 +3193,48 @@
         <v>6.2650617790504253</v>
       </c>
       <c r="I32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.6915666803436149</v>
       </c>
       <c r="J32">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K32">
         <f t="shared" si="5"/>
-        <v>3.4331333606872294E-2</v>
+        <v>1.7415666803436151E-2</v>
       </c>
       <c r="L32">
-        <f t="shared" si="14"/>
-        <v>0.91244078234646742</v>
+        <f t="shared" si="15"/>
+        <v>1.7986855886029911</v>
       </c>
       <c r="M32">
-        <f t="shared" si="15"/>
-        <v>0.24635901123354623</v>
-      </c>
-    </row>
-    <row r="33" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.48564510892280766</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="8"/>
+        <v>0.48564510892280766</v>
+      </c>
+    </row>
+    <row r="33" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C33">
         <v>0.28000000000000003</v>
       </c>
       <c r="D33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="F33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.56</v>
       </c>
       <c r="G33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.31819177941838417</v>
       </c>
       <c r="H33">
@@ -2989,44 +3242,48 @@
         <v>6.3638355883676834</v>
       </c>
       <c r="I33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.7818739647429516</v>
       </c>
       <c r="J33">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K33">
         <f t="shared" si="5"/>
-        <v>3.6137479294859033E-2</v>
+        <v>1.8318739647429517E-2</v>
       </c>
       <c r="L33">
-        <f t="shared" si="14"/>
-        <v>0.88050352605432158</v>
+        <f t="shared" si="15"/>
+        <v>1.7369741889586428</v>
       </c>
       <c r="M33">
-        <f t="shared" si="15"/>
-        <v>0.24654098729521007</v>
-      </c>
-    </row>
-    <row r="34" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.48635277290841999</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="8"/>
+        <v>0.48635277290841999</v>
+      </c>
+    </row>
+    <row r="34" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C34">
         <v>0.28999999999999998</v>
       </c>
       <c r="D34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="F34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.58</v>
       </c>
       <c r="G34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.32296882782654257</v>
       </c>
       <c r="H34">
@@ -3034,44 +3291,48 @@
         <v>6.4593765565308514</v>
       </c>
       <c r="I34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.8732192013939468</v>
       </c>
       <c r="J34">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K34">
         <f t="shared" si="5"/>
-        <v>3.7964384027878932E-2</v>
+        <v>1.923219201393947E-2</v>
       </c>
       <c r="L34">
-        <f t="shared" si="14"/>
-        <v>0.85071531145974144</v>
+        <f t="shared" si="15"/>
+        <v>1.6793136611388613</v>
       </c>
       <c r="M34">
-        <f t="shared" si="15"/>
-        <v>0.24670744032332501</v>
-      </c>
-    </row>
-    <row r="35" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.48700096173026974</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="8"/>
+        <v>0.48700096173026974</v>
+      </c>
+    </row>
+    <row r="35" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C35">
         <v>0.3</v>
       </c>
       <c r="D35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.3</v>
       </c>
       <c r="F35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.6</v>
       </c>
       <c r="G35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.32759267427611211</v>
       </c>
       <c r="H35">
@@ -3079,44 +3340,48 @@
         <v>6.5518534855222423</v>
       </c>
       <c r="I35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.9655560456566725</v>
       </c>
       <c r="J35">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K35">
         <f t="shared" si="5"/>
-        <v>3.9811120913133449E-2</v>
+        <v>2.0155560456566725E-2</v>
       </c>
       <c r="L35">
-        <f t="shared" si="14"/>
-        <v>0.8228672460413976</v>
+        <f t="shared" si="15"/>
+        <v>1.6253215830045635</v>
       </c>
       <c r="M35">
-        <f t="shared" si="15"/>
-        <v>0.24686017381241926</v>
-      </c>
-    </row>
-    <row r="36" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.48759647490136904</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="8"/>
+        <v>0.48759647490136904</v>
+      </c>
+    </row>
+    <row r="36" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C36">
         <v>0.31</v>
       </c>
       <c r="D36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.31</v>
       </c>
       <c r="F36">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.62</v>
       </c>
       <c r="G36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.33207112962159829</v>
       </c>
       <c r="H36">
@@ -3124,44 +3389,48 @@
         <v>6.6414225924319652</v>
       </c>
       <c r="I36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.0588410036539093</v>
       </c>
       <c r="J36">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K36">
         <f t="shared" si="5"/>
-        <v>4.1676820073078186E-2</v>
+        <v>2.1088410036539093E-2</v>
       </c>
       <c r="L36">
-        <f t="shared" si="14"/>
-        <v>0.79677655118439561</v>
+        <f t="shared" si="15"/>
+        <v>1.5746617646670904</v>
       </c>
       <c r="M36">
-        <f t="shared" si="15"/>
-        <v>0.24700073086716265</v>
-      </c>
-    </row>
-    <row r="37" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.48814514704679801</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="8"/>
+        <v>0.48814514704679801</v>
+      </c>
+    </row>
+    <row r="37" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C37">
         <v>0.32</v>
       </c>
       <c r="D37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.32</v>
       </c>
       <c r="F37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.6400000000000001</v>
       </c>
       <c r="G37">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.33641143808612001</v>
       </c>
       <c r="H37">
@@ -3169,44 +3438,48 @@
         <v>6.7282287617224004</v>
       </c>
       <c r="I37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.1530332037511681</v>
       </c>
       <c r="J37">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K37">
         <f t="shared" si="5"/>
-        <v>4.3560664075023361E-2</v>
+        <v>2.2030332037511681E-2</v>
       </c>
       <c r="L37">
-        <f t="shared" si="14"/>
-        <v>0.77228262063849085</v>
+        <f t="shared" si="15"/>
+        <v>1.5270375294993401</v>
       </c>
       <c r="M37">
-        <f t="shared" si="15"/>
-        <v>0.24713043860431708</v>
-      </c>
-    </row>
-    <row r="38" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.48865200943978887</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="8"/>
+        <v>0.48865200943978887</v>
+      </c>
+    </row>
+    <row r="38" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C38">
         <v>0.33</v>
       </c>
       <c r="D38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.33</v>
       </c>
       <c r="F38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.6600000000000001</v>
       </c>
       <c r="G38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.34062033198365266</v>
       </c>
       <c r="H38">
@@ -3214,44 +3487,48 @@
         <v>6.8124066396730534</v>
       </c>
       <c r="I38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.2480941910921075</v>
       </c>
       <c r="J38">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K38">
         <f t="shared" si="5"/>
-        <v>4.5461883821842151E-2</v>
+        <v>2.2980941910921072E-2</v>
       </c>
       <c r="L38">
-        <f t="shared" si="14"/>
-        <v>0.7492437693925954</v>
+        <f t="shared" si="15"/>
+        <v>1.4821861231970743</v>
       </c>
       <c r="M38">
-        <f t="shared" si="15"/>
-        <v>0.2472504438995565</v>
-      </c>
-    </row>
-    <row r="39" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.48912142065503456</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="8"/>
+        <v>0.48912142065503456</v>
+      </c>
+    </row>
+    <row r="39" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C39">
         <v>0.34</v>
       </c>
       <c r="D39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.34</v>
       </c>
       <c r="F39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.6800000000000002</v>
       </c>
       <c r="G39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.34470407975589484</v>
       </c>
       <c r="H39">
@@ -3259,44 +3536,48 @@
         <v>6.8940815951178971</v>
       </c>
       <c r="I39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.3439877423400852</v>
       </c>
       <c r="J39">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K39">
         <f t="shared" si="5"/>
-        <v>4.7379754846801701E-2</v>
+        <v>2.3939877423400851E-2</v>
       </c>
       <c r="L39">
-        <f t="shared" si="14"/>
-        <v>0.72753453636572285</v>
+        <f t="shared" si="15"/>
+        <v>1.4398740380305877</v>
       </c>
       <c r="M39">
-        <f t="shared" si="15"/>
-        <v>0.2473617423643458</v>
-      </c>
-    </row>
-    <row r="40" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.48955717293039985</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="8"/>
+        <v>0.48955717293039985</v>
+      </c>
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C40">
         <v>0.35</v>
       </c>
       <c r="D40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.35</v>
       </c>
       <c r="F40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.7</v>
       </c>
       <c r="G40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.34866852831389705</v>
       </c>
       <c r="H40">
@@ -3304,44 +3585,48 @@
         <v>6.9733705662779411</v>
       </c>
       <c r="I40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.4406796981972794</v>
       </c>
       <c r="J40">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K40">
         <f t="shared" si="5"/>
-        <v>4.9313593963945586E-2</v>
+        <v>2.4906796981972793E-2</v>
       </c>
       <c r="L40">
-        <f t="shared" si="14"/>
-        <v>0.70704343424820626</v>
+        <f t="shared" si="15"/>
+        <v>1.3998930836681194</v>
       </c>
       <c r="M40">
-        <f t="shared" si="15"/>
-        <v>0.24746520198687216</v>
-      </c>
-    </row>
-    <row r="41" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.48996257928384174</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="8"/>
+        <v>0.48996257928384174</v>
+      </c>
+    </row>
+    <row r="41" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>0.36</v>
       </c>
       <c r="D41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.36</v>
       </c>
       <c r="F41">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.72</v>
       </c>
       <c r="G41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.35251914050292288</v>
       </c>
       <c r="H41">
@@ -3349,44 +3634,48 @@
         <v>7.0503828100584576</v>
       </c>
       <c r="I41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.5381378116210445</v>
       </c>
       <c r="J41">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K41">
         <f t="shared" si="5"/>
-        <v>5.1262756232420888E-2</v>
+        <v>2.5881378116210444E-2</v>
       </c>
       <c r="L41">
-        <f t="shared" si="14"/>
-        <v>0.6876710626027045</v>
+        <f t="shared" si="15"/>
+        <v>1.3620570702227304</v>
       </c>
       <c r="M41">
-        <f t="shared" si="15"/>
-        <v>0.24756158253697361</v>
-      </c>
-    </row>
-    <row r="42" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.49034054528018289</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="8"/>
+        <v>0.49034054528018289</v>
+      </c>
+    </row>
+    <row r="42" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C42">
         <v>0.37</v>
       </c>
       <c r="D42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.37</v>
       </c>
       <c r="F42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.74</v>
       </c>
       <c r="G42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.35626102837124329</v>
       </c>
       <c r="H42">
@@ -3394,44 +3683,48 @@
         <v>7.1252205674248659</v>
       </c>
       <c r="I42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.6363316099472005</v>
       </c>
       <c r="J42">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K42">
         <f t="shared" si="5"/>
-        <v>5.322663219894401E-2</v>
+        <v>2.6863316099472005E-2</v>
       </c>
       <c r="L42">
-        <f t="shared" si="14"/>
-        <v>0.66932851779848535</v>
+        <f t="shared" si="15"/>
+        <v>1.3261989958799076</v>
       </c>
       <c r="M42">
-        <f t="shared" si="15"/>
-        <v>0.24765155158543958</v>
-      </c>
-    </row>
-    <row r="43" spans="3:13" x14ac:dyDescent="0.3">
+        <f t="shared" si="16"/>
+        <v>0.4906936284755658</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="8"/>
+        <v>0.4906936284755658</v>
+      </c>
+    </row>
+    <row r="43" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C43">
         <v>0.38</v>
       </c>
       <c r="D43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E43">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.38</v>
       </c>
       <c r="F43">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.76</v>
       </c>
       <c r="G43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.35989898281221949</v>
       </c>
       <c r="H43">
@@ -3439,24 +3732,28 @@
         <v>7.1979796562443896</v>
       </c>
       <c r="I43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.7352322693728679</v>
       </c>
       <c r="J43">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="10"/>
+        <v>0.5</v>
       </c>
       <c r="K43">
         <f t="shared" si="5"/>
-        <v>5.5204645387457354E-2</v>
+        <v>2.7852322693728677E-2</v>
       </c>
       <c r="L43">
-        <f t="shared" si="14"/>
-        <v>0.65193604684215489</v>
+        <f t="shared" si="15"/>
+        <v>1.2921686523948523</v>
       </c>
       <c r="M43">
-        <f t="shared" si="15"/>
-        <v>0.24773569780001886</v>
+        <f t="shared" si="16"/>
+        <v>0.49102408791004387</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="8"/>
+        <v>0.49102408791004387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
// v 6.88 beta, see fixesandbugs.txt
</commit_message>
<xml_diff>
--- a/auxfiles/cukvertN.xlsx
+++ b/auxfiles/cukvertN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prgc\lisemgit\openlisem\auxfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1068727F-8105-4BCC-BBCB-2B9FE0EE2FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624478A1-901C-43D9-95C5-73E5014AD690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{E7372BA5-4E66-4B5A-980A-99B2857E7BC6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>h</t>
   </si>
@@ -63,6 +63,21 @@
   </si>
   <si>
     <t>n*(0.1+Q/qmax)</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>pram</t>
+  </si>
+  <si>
+    <t>Qest</t>
+  </si>
+  <si>
+    <t>Qmin</t>
   </si>
 </sst>
 </file>
@@ -189,118 +204,118 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -334,118 +349,118 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>7.7427380074318139E-2</c:v>
+                  <c:v>5.2985769829245202E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18238490530892423</c:v>
+                  <c:v>0.1294604828406635</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.26353119432340594</c:v>
+                  <c:v>0.19260675932189014</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.32000000000000006</c:v>
+                  <c:v>0.23880597014925378</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35904806348847795</c:v>
+                  <c:v>0.27190806354677599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.38663726473607829</c:v>
+                  <c:v>0.2958925368598187</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.4066815273330876</c:v>
+                  <c:v>0.31363793658159167</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.42164871285155531</c:v>
+                  <c:v>0.32706847585371679</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.43310632925738418</c:v>
+                  <c:v>0.33745560573382399</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.44207215960481672</c:v>
+                  <c:v>0.34564865562159053</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.4492243621368664</c:v>
+                  <c:v>0.35222569595591413</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.45502658876385088</c:v>
+                  <c:v>0.3575884814787394</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.45980360061021947</c:v>
+                  <c:v>0.36202208673366826</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.46378798003267263</c:v>
+                  <c:v>0.36573281443453415</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.46714968496854481</c:v>
+                  <c:v>0.36887271402988014</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.47001519535254632</c:v>
+                  <c:v>0.37155574570183364</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.47248019927747331</c:v>
+                  <c:v>0.37386864319908264</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.47461817729277561</c:v>
+                  <c:v>0.3758783507707219</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.47648632528202672</c:v>
+                  <c:v>0.37763720486696284</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.47812971504504997</c:v>
+                  <c:v>0.37918660440030605</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.47958426562589512</c:v>
+                  <c:v>0.38055965060461777</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.48087889785010607</c:v>
+                  <c:v>0.38178307302472247</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.48203711866127152</c:v>
+                  <c:v>0.38287865340174221</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.48307820134138307</c:v>
+                  <c:v>0.3838642913727694</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.48401807528266633</c:v>
+                  <c:v>0.38475481125489008</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.48487000427381877</c:v>
+                  <c:v>0.38556257934797089</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.48564510892280766</c:v>
+                  <c:v>0.38629798096222534</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.48635277290841999</c:v>
+                  <c:v>0.3869697924725542</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.48700096173026974</c:v>
+                  <c:v>0.38758547402038274</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.48759647490136904</c:v>
+                  <c:v>0.3881514016600715</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.48814514704679801</c:v>
+                  <c:v>0.3886730528819235</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.48865200943978887</c:v>
+                  <c:v>0.38915515593741695</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.48912142065503456</c:v>
+                  <c:v>0.38960181083916512</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.48955717293039985</c:v>
+                  <c:v>0.39001658803108624</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.48996257928384174</c:v>
+                  <c:v>0.39040260933165438</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.49034054528018289</c:v>
+                  <c:v>0.3907626147109472</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.4906936284755658</c:v>
+                  <c:v>0.39109901767591937</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.49102408791004387</c:v>
+                  <c:v>0.39141395144047025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -479,118 +494,118 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>9.1614288791279658E-3</c:v>
+                  <c:v>3.053809626375989E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8711624283209614E-2</c:v>
+                  <c:v>9.570541427736539E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.57221899881001E-2</c:v>
+                  <c:v>1.8574063329366702E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.8888888888888906E-2</c:v>
+                  <c:v>2.9629629629629641E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.12736542412069948</c:v>
+                  <c:v>4.2455141373566485E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17053102319555966</c:v>
+                  <c:v>5.6843674398519888E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.21789979824502809</c:v>
+                  <c:v>7.2633266081676029E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.26907580474887255</c:v>
+                  <c:v>8.969193491629085E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.32372743523361935</c:v>
+                  <c:v>0.10790914507787314</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.38157141418444396</c:v>
+                  <c:v>0.12719047139481465</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.44236210616177418</c:v>
+                  <c:v>0.14745403538725807</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.50588400596807026</c:v>
+                  <c:v>0.16862800198935676</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.57194625338397864</c:v>
+                  <c:v>0.1906487511279929</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.64037849925402024</c:v>
+                  <c:v>0.21345949975134007</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.71102770935565829</c:v>
+                  <c:v>0.2370092364518861</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.78375564036309164</c:v>
+                  <c:v>0.26125188012103057</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.85843681071919919</c:v>
+                  <c:v>0.2861456035730664</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.93495684444617699</c:v>
+                  <c:v>0.31165228148205903</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.0132111016186967</c:v>
+                  <c:v>0.33773703387289888</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.0931035330127941</c:v>
+                  <c:v>0.36436784433759811</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.1745457127278149</c:v>
+                  <c:v>0.39151523757593831</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.2574560139902171</c:v>
+                  <c:v>0.41915200466340569</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.341758901513163</c:v>
+                  <c:v>0.44725296717105434</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.4273843197377576</c:v>
+                  <c:v>0.47579477324591918</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.5142671606934499</c:v>
+                  <c:v>0.50475572023115001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.6023467985347395</c:v>
+                  <c:v>0.53411559951157983</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.6915666803436149</c:v>
+                  <c:v>0.5638555601145383</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.7818739647429516</c:v>
+                  <c:v>0.59395798824765056</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.8732192013939468</c:v>
+                  <c:v>0.62440640046464901</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.9655560456566725</c:v>
+                  <c:v>0.65518534855222421</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.0588410036539093</c:v>
+                  <c:v>0.68628033455130311</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.1530332037511681</c:v>
+                  <c:v>0.71767773458372275</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.2480941910921075</c:v>
+                  <c:v>0.74936473036403595</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3439877423400852</c:v>
+                  <c:v>0.78132924744669507</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.4406796981972794</c:v>
+                  <c:v>0.81355989939909312</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.5381378116210445</c:v>
+                  <c:v>0.84604593720701493</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.6363316099472005</c:v>
+                  <c:v>0.8787772033157335</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.7352322693728679</c:v>
+                  <c:v>0.911744089790956</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -624,118 +639,118 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>9.1614288791279658E-3</c:v>
+                  <c:v>3.053809626375989E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8711624283209614E-2</c:v>
+                  <c:v>9.570541427736539E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.57221899881001E-2</c:v>
+                  <c:v>1.8574063329366702E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.8888888888888906E-2</c:v>
+                  <c:v>2.9629629629629641E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.12736542412069948</c:v>
+                  <c:v>4.2455141373566485E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17053102319555966</c:v>
+                  <c:v>5.6843674398519888E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.21789979824502809</c:v>
+                  <c:v>7.2633266081676029E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.26907580474887255</c:v>
+                  <c:v>8.969193491629085E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.32372743523361935</c:v>
+                  <c:v>0.10790914507787314</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.38157141418444396</c:v>
+                  <c:v>0.12719047139481465</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.44236210616177418</c:v>
+                  <c:v>0.14745403538725807</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.45502658876385088</c:v>
+                  <c:v>0.16862800198935676</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.45980360061021947</c:v>
+                  <c:v>0.1906487511279929</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.46378798003267263</c:v>
+                  <c:v>0.21345949975134007</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.46714968496854481</c:v>
+                  <c:v>0.2370092364518861</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.47001519535254632</c:v>
+                  <c:v>0.26125188012103057</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.47248019927747331</c:v>
+                  <c:v>0.2861456035730664</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.47461817729277561</c:v>
+                  <c:v>0.31165228148205903</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.47648632528202672</c:v>
+                  <c:v>0.33773703387289888</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.47812971504504997</c:v>
+                  <c:v>0.36436784433759811</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.47958426562589512</c:v>
+                  <c:v>0.38055965060461777</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.48087889785010607</c:v>
+                  <c:v>0.38178307302472247</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.48203711866127152</c:v>
+                  <c:v>0.38287865340174221</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.48307820134138307</c:v>
+                  <c:v>0.3838642913727694</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.48401807528266633</c:v>
+                  <c:v>0.38475481125489008</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.48487000427381877</c:v>
+                  <c:v>0.38556257934797089</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.48564510892280766</c:v>
+                  <c:v>0.38629798096222534</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.48635277290841999</c:v>
+                  <c:v>0.3869697924725542</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.48700096173026974</c:v>
+                  <c:v>0.38758547402038274</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.48759647490136904</c:v>
+                  <c:v>0.3881514016600715</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.48814514704679801</c:v>
+                  <c:v>0.3886730528819235</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.48865200943978887</c:v>
+                  <c:v>0.38915515593741695</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.48912142065503456</c:v>
+                  <c:v>0.38960181083916512</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.48955717293039985</c:v>
+                  <c:v>0.39001658803108624</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.48996257928384174</c:v>
+                  <c:v>0.39040260933165438</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.49034054528018289</c:v>
+                  <c:v>0.3907626147109472</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.4906936284755658</c:v>
+                  <c:v>0.39109901767591937</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.49102408791004387</c:v>
+                  <c:v>0.39141395144047025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -743,7 +758,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-278B-4E11-995B-DD5CE8EF9A3F}"/>
+              <c16:uniqueId val="{00000000-5436-4A06-8B47-66DDDD29DBCE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1508,16 +1523,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1842,10 +1857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCF5D42-AFF0-4820-B50F-3BBD607733D8}">
-  <dimension ref="C3:N43"/>
+  <dimension ref="C2:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N43" sqref="N6:N43"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1854,12 +1869,26 @@
     <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
       <c r="H3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
       <c r="H4">
         <v>0.01</v>
       </c>
@@ -1880,9 +1909,6 @@
       <c r="G5" t="s">
         <v>7</v>
       </c>
-      <c r="H5">
-        <v>5.0000000000000001E-3</v>
-      </c>
       <c r="I5" t="s">
         <v>4</v>
       </c>
@@ -1894,6 +1920,12 @@
       </c>
       <c r="L5" t="s">
         <v>6</v>
+      </c>
+      <c r="M5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.3">
@@ -1916,31 +1948,31 @@
         <v>4.5807144395639827E-2</v>
       </c>
       <c r="H6">
-        <f>G6*SQRT($H$4)/$H$5</f>
-        <v>0.91614288791279652</v>
+        <f>G6*SQRT($H$4)/$H$2</f>
+        <v>0.3053809626375989</v>
       </c>
       <c r="I6">
         <f>H6*E6</f>
-        <v>9.1614288791279658E-3</v>
+        <v>3.053809626375989E-3</v>
       </c>
       <c r="J6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K6">
-        <f>($H$3+I6/J6)*$H$5</f>
-        <v>5.916142887912797E-4</v>
+        <f>($H$3+I6/J6)*$H$2</f>
+        <v>8.6451786098909955E-4</v>
       </c>
       <c r="L6">
         <f>G6*SQRT($H$4)/K6</f>
-        <v>7.7427380074318144</v>
+        <v>5.2985769829245202</v>
       </c>
       <c r="M6">
         <f>L6*E6</f>
-        <v>7.7427380074318139E-2</v>
+        <v>5.2985769829245202E-2</v>
       </c>
       <c r="N6">
         <f>MIN(M6,I6)</f>
-        <v>9.1614288791279658E-3</v>
+        <v>3.053809626375989E-3</v>
       </c>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
@@ -1964,32 +1996,32 @@
         <v>7.1779060708024034E-2</v>
       </c>
       <c r="H7">
-        <f t="shared" ref="H7:H43" si="3">G7*SQRT($H$4)/$H$5</f>
-        <v>1.4355812141604807</v>
+        <f>G7*SQRT($H$4)/$H$2</f>
+        <v>0.47852707138682693</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:I27" si="4">H7*E7</f>
-        <v>2.8711624283209614E-2</v>
+        <f t="shared" ref="I7:I27" si="3">H7*E7</f>
+        <v>9.570541427736539E-3</v>
       </c>
       <c r="J7">
         <f>J6</f>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K7:K43" si="5">($H$3+I7/J7)*$H$5</f>
-        <v>7.8711624283209615E-4</v>
+        <f>($H$3+I7/J7)*$H$2</f>
+        <v>1.1088953035401203E-3</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7:L27" si="6">G7*SQRT($H$4)/K7</f>
-        <v>9.1192452654462119</v>
+        <f t="shared" ref="L7:L27" si="4">G7*SQRT($H$4)/K7</f>
+        <v>6.4730241420331742</v>
       </c>
       <c r="M7">
-        <f t="shared" ref="M7:M27" si="7">L7*E7</f>
-        <v>0.18238490530892423</v>
+        <f t="shared" ref="M7:M27" si="5">L7*E7</f>
+        <v>0.1294604828406635</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="N7:N43" si="8">MIN(M7,I7)</f>
-        <v>2.8711624283209614E-2</v>
+        <f t="shared" ref="N7:N43" si="6">MIN(M7,I7)</f>
+        <v>9.570541427736539E-3</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
@@ -1997,7 +2029,7 @@
         <v>0.03</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D43" si="9">D7</f>
+        <f t="shared" ref="D8:D43" si="7">D7</f>
         <v>1</v>
       </c>
       <c r="E8">
@@ -2013,32 +2045,32 @@
         <v>9.2870316646833512E-2</v>
       </c>
       <c r="H8">
+        <f>G8*SQRT($H$4)/$H$2</f>
+        <v>0.61913544431222345</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="3"/>
-        <v>1.8574063329366701</v>
-      </c>
-      <c r="I8">
+        <v>1.8574063329366702E-2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8:J43" si="8">J7</f>
+        <v>0.4</v>
+      </c>
+      <c r="K8">
+        <f>($H$3+I8/J8)*$H$2</f>
+        <v>1.4465273748512514E-3</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="4"/>
-        <v>5.57221899881001E-2</v>
-      </c>
-      <c r="J8">
-        <f t="shared" ref="J8:J43" si="10">J7</f>
-        <v>0.5</v>
-      </c>
-      <c r="K8">
+        <v>6.4202253107296716</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="5"/>
-        <v>1.057221899881001E-3</v>
-      </c>
-      <c r="L8">
+        <v>0.19260675932189014</v>
+      </c>
+      <c r="N8">
         <f t="shared" si="6"/>
-        <v>8.7843731441135322</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="7"/>
-        <v>0.26353119432340594</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="8"/>
-        <v>5.57221899881001E-2</v>
+        <v>1.8574063329366702E-2</v>
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.3">
@@ -2046,7 +2078,7 @@
         <v>0.04</v>
       </c>
       <c r="D9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E9">
@@ -2062,32 +2094,32 @@
         <v>0.11111111111111115</v>
       </c>
       <c r="H9">
+        <f>G9*SQRT($H$4)/$H$2</f>
+        <v>0.74074074074074103</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="3"/>
-        <v>2.2222222222222228</v>
-      </c>
-      <c r="I9">
+        <v>2.9629629629629641E-2</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K9">
+        <f>($H$3+I9/J9)*$H$2</f>
+        <v>1.8611111111111113E-3</v>
+      </c>
+      <c r="L9">
         <f t="shared" si="4"/>
-        <v>8.8888888888888906E-2</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K9">
+        <v>5.9701492537313445</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="5"/>
-        <v>1.3888888888888889E-3</v>
-      </c>
-      <c r="L9">
+        <v>0.23880597014925378</v>
+      </c>
+      <c r="N9">
         <f t="shared" si="6"/>
-        <v>8.0000000000000018</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="7"/>
-        <v>0.32000000000000006</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="8"/>
-        <v>8.8888888888888906E-2</v>
+        <v>2.9629629629629641E-2</v>
       </c>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.3">
@@ -2095,7 +2127,7 @@
         <v>0.05</v>
       </c>
       <c r="D10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E10">
@@ -2111,32 +2143,32 @@
         <v>0.12736542412069946</v>
       </c>
       <c r="H10">
+        <f>G10*SQRT($H$4)/$H$2</f>
+        <v>0.8491028274713297</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="3"/>
-        <v>2.5473084824139893</v>
-      </c>
-      <c r="I10">
+        <v>4.2455141373566485E-2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K10">
+        <f>($H$3+I10/J10)*$H$2</f>
+        <v>2.3420678015087433E-3</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="4"/>
-        <v>0.12736542412069948</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K10">
+        <v>5.4381612709355194</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="5"/>
-        <v>1.7736542412069951E-3</v>
-      </c>
-      <c r="L10">
+        <v>0.27190806354677599</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="6"/>
-        <v>7.1809612697695586</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="7"/>
-        <v>0.35904806348847795</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="8"/>
-        <v>0.12736542412069948</v>
+        <v>4.2455141373566485E-2</v>
       </c>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.3">
@@ -2144,7 +2176,7 @@
         <v>0.06</v>
       </c>
       <c r="D11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E11">
@@ -2160,32 +2192,32 @@
         <v>0.14210918599629971</v>
       </c>
       <c r="H11">
+        <f>G11*SQRT($H$4)/$H$2</f>
+        <v>0.94739457330866483</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="3"/>
-        <v>2.8421837199259943</v>
-      </c>
-      <c r="I11">
+        <v>5.6843674398519888E-2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K11">
+        <f>($H$3+I11/J11)*$H$2</f>
+        <v>2.8816377899444959E-3</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="4"/>
-        <v>0.17053102319555966</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K11">
+        <v>4.9315422809969789</v>
+      </c>
+      <c r="M11">
         <f t="shared" si="5"/>
-        <v>2.2053102319555969E-3</v>
-      </c>
-      <c r="L11">
+        <v>0.2958925368598187</v>
+      </c>
+      <c r="N11">
         <f t="shared" si="6"/>
-        <v>6.4439544122679715</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="7"/>
-        <v>0.38663726473607829</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="8"/>
-        <v>0.17053102319555966</v>
+        <v>5.6843674398519888E-2</v>
       </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
@@ -2193,7 +2225,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E12">
@@ -2209,32 +2241,32 @@
         <v>0.1556427130321629</v>
       </c>
       <c r="H12">
+        <f>G12*SQRT($H$4)/$H$2</f>
+        <v>1.037618086881086</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="3"/>
-        <v>3.1128542606432581</v>
-      </c>
-      <c r="I12">
+        <v>7.2633266081676029E-2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K12">
+        <f>($H$3+I12/J12)*$H$2</f>
+        <v>3.4737474780628511E-3</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="4"/>
-        <v>0.21789979824502809</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K12">
+        <v>4.4805419511655948</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="5"/>
-        <v>2.6789979824502807E-3</v>
-      </c>
-      <c r="L12">
+        <v>0.31363793658159167</v>
+      </c>
+      <c r="N12">
         <f t="shared" si="6"/>
-        <v>5.809736104758394</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="7"/>
-        <v>0.4066815273330876</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="8"/>
-        <v>0.21789979824502809</v>
+        <v>7.2633266081676029E-2</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
@@ -2242,7 +2274,7 @@
         <v>0.08</v>
       </c>
       <c r="D13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E13">
@@ -2258,32 +2290,32 @@
         <v>0.16817237796804532</v>
       </c>
       <c r="H13">
+        <f>G13*SQRT($H$4)/$H$2</f>
+        <v>1.1211491864536356</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="3"/>
-        <v>3.3634475593609068</v>
-      </c>
-      <c r="I13">
+        <v>8.969193491629085E-2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K13">
+        <f>($H$3+I13/J13)*$H$2</f>
+        <v>4.1134475593609067E-3</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="4"/>
-        <v>0.26907580474887255</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K13">
+        <v>4.0883559481714595</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="5"/>
-        <v>3.1907580474887253E-3</v>
-      </c>
-      <c r="L13">
+        <v>0.32706847585371679</v>
+      </c>
+      <c r="N13">
         <f t="shared" si="6"/>
-        <v>5.2706089106444409</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="7"/>
-        <v>0.42164871285155531</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="8"/>
-        <v>0.26907580474887255</v>
+        <v>8.969193491629085E-2</v>
       </c>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.3">
@@ -2291,7 +2323,7 @@
         <v>0.09</v>
       </c>
       <c r="D14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E14">
@@ -2307,32 +2339,32 @@
         <v>0.17984857512978852</v>
       </c>
       <c r="H14">
+        <f>G14*SQRT($H$4)/$H$2</f>
+        <v>1.198990500865257</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="3"/>
-        <v>3.5969715025957707</v>
-      </c>
-      <c r="I14">
+        <v>0.10790914507787314</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K14">
+        <f>($H$3+I14/J14)*$H$2</f>
+        <v>4.7965929404202422E-3</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="4"/>
-        <v>0.32372743523361935</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K14">
+        <v>3.7495067303758223</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="5"/>
-        <v>3.7372743523361937E-3</v>
-      </c>
-      <c r="L14">
+        <v>0.33745560573382399</v>
+      </c>
+      <c r="N14">
         <f t="shared" si="6"/>
-        <v>4.8122925473042688</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="7"/>
-        <v>0.43310632925738418</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="8"/>
-        <v>0.32372743523361935</v>
+        <v>0.10790914507787314</v>
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.3">
@@ -2340,7 +2372,7 @@
         <v>0.1</v>
       </c>
       <c r="D15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E15">
@@ -2356,32 +2388,32 @@
         <v>0.19078570709222198</v>
       </c>
       <c r="H15">
+        <f>G15*SQRT($H$4)/$H$2</f>
+        <v>1.2719047139481465</v>
+      </c>
+      <c r="I15">
         <f t="shared" si="3"/>
-        <v>3.8157141418444396</v>
-      </c>
-      <c r="I15">
+        <v>0.12719047139481465</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K15">
+        <f>($H$3+I15/J15)*$H$2</f>
+        <v>5.5196426773055493E-3</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="4"/>
-        <v>0.38157141418444396</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K15">
+        <v>3.4564865562159053</v>
+      </c>
+      <c r="M15">
         <f t="shared" si="5"/>
-        <v>4.3157141418444398E-3</v>
-      </c>
-      <c r="L15">
+        <v>0.34564865562159053</v>
+      </c>
+      <c r="N15">
         <f t="shared" si="6"/>
-        <v>4.4207215960481667</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="7"/>
-        <v>0.44207215960481672</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="8"/>
-        <v>0.38157141418444396</v>
+        <v>0.12719047139481465</v>
       </c>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.3">
@@ -2389,7 +2421,7 @@
         <v>0.11</v>
       </c>
       <c r="D16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E16">
@@ -2405,32 +2437,32 @@
         <v>0.20107368461898828</v>
       </c>
       <c r="H16">
+        <f>G16*SQRT($H$4)/$H$2</f>
+        <v>1.3404912307932553</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="3"/>
-        <v>4.0214736923797654</v>
-      </c>
-      <c r="I16">
+        <v>0.14745403538725807</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K16">
+        <f>($H$3+I16/J16)*$H$2</f>
+        <v>6.2795263270221764E-3</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="4"/>
-        <v>0.44236210616177418</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K16">
+        <v>3.202051781417401</v>
+      </c>
+      <c r="M16">
         <f t="shared" si="5"/>
-        <v>4.9236210616177417E-3</v>
-      </c>
-      <c r="L16">
+        <v>0.35222569595591413</v>
+      </c>
+      <c r="N16">
         <f t="shared" si="6"/>
-        <v>4.0838578376078765</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="7"/>
-        <v>0.4492243621368664</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="8"/>
-        <v>0.44236210616177418</v>
+        <v>0.14745403538725807</v>
       </c>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.3">
@@ -2438,7 +2470,7 @@
         <v>0.12</v>
       </c>
       <c r="D17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E17">
@@ -2454,32 +2486,32 @@
         <v>0.21078500248669593</v>
       </c>
       <c r="H17">
+        <f>G17*SQRT($H$4)/$H$2</f>
+        <v>1.4052333499113063</v>
+      </c>
+      <c r="I17">
         <f t="shared" si="3"/>
-        <v>4.2157000497339192</v>
-      </c>
-      <c r="I17">
+        <v>0.16862800198935676</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K17">
+        <f>($H$3+I17/J17)*$H$2</f>
+        <v>7.0735500746008772E-3</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="4"/>
-        <v>0.50588400596807026</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K17">
+        <v>2.9799040123228284</v>
+      </c>
+      <c r="M17">
         <f t="shared" si="5"/>
-        <v>5.5588400596807029E-3</v>
-      </c>
-      <c r="L17">
+        <v>0.3575884814787394</v>
+      </c>
+      <c r="N17">
         <f t="shared" si="6"/>
-        <v>3.7918882396987574</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="7"/>
-        <v>0.45502658876385088</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="8"/>
-        <v>0.45502658876385088</v>
+        <v>0.16862800198935676</v>
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.3">
@@ -2487,7 +2519,7 @@
         <v>0.13</v>
       </c>
       <c r="D18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E18">
@@ -2503,32 +2535,32 @@
         <v>0.21997932822460714</v>
       </c>
       <c r="H18">
+        <f>G18*SQRT($H$4)/$H$2</f>
+        <v>1.4665288548307145</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="3"/>
-        <v>4.399586564492143</v>
-      </c>
-      <c r="I18">
+        <v>0.1906487511279929</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K18">
+        <f>($H$3+I18/J18)*$H$2</f>
+        <v>7.8993281672997337E-3</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="4"/>
-        <v>0.57194625338397864</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K18">
+        <v>2.7847852825666788</v>
+      </c>
+      <c r="M18">
         <f t="shared" si="5"/>
-        <v>6.2194625338397869E-3</v>
-      </c>
-      <c r="L18">
+        <v>0.36202208673366826</v>
+      </c>
+      <c r="N18">
         <f t="shared" si="6"/>
-        <v>3.5369507739247652</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="7"/>
-        <v>0.45980360061021947</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="8"/>
-        <v>0.45980360061021947</v>
+        <v>0.1906487511279929</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.3">
@@ -2536,7 +2568,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="D19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E19">
@@ -2552,32 +2584,32 @@
         <v>0.22870660687643574</v>
       </c>
       <c r="H19">
+        <f>G19*SQRT($H$4)/$H$2</f>
+        <v>1.5247107125095718</v>
+      </c>
+      <c r="I19">
         <f t="shared" si="3"/>
-        <v>4.5741321375287152</v>
-      </c>
-      <c r="I19">
+        <v>0.21345949975134007</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K19">
+        <f>($H$3+I19/J19)*$H$2</f>
+        <v>8.7547312406752523E-3</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="4"/>
-        <v>0.64037849925402024</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K19">
+        <v>2.6123772459609578</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="5"/>
-        <v>6.9037849925402033E-3</v>
-      </c>
-      <c r="L19">
+        <v>0.36573281443453415</v>
+      </c>
+      <c r="N19">
         <f t="shared" si="6"/>
-        <v>3.3127712859476612</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="7"/>
-        <v>0.46378798003267263</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="8"/>
-        <v>0.46378798003267263</v>
+        <v>0.21345949975134007</v>
       </c>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.3">
@@ -2585,7 +2617,7 @@
         <v>0.15</v>
       </c>
       <c r="D20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E20">
@@ -2601,32 +2633,32 @@
         <v>0.2370092364518861</v>
       </c>
       <c r="H20">
+        <f>G20*SQRT($H$4)/$H$2</f>
+        <v>1.5800615763459074</v>
+      </c>
+      <c r="I20">
         <f t="shared" si="3"/>
-        <v>4.7401847290377219</v>
-      </c>
-      <c r="I20">
+        <v>0.2370092364518861</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K20">
+        <f>($H$3+I20/J20)*$H$2</f>
+        <v>9.6378463669457293E-3</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="4"/>
-        <v>0.71102770935565829</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K20">
+        <v>2.4591514268658679</v>
+      </c>
+      <c r="M20">
         <f t="shared" si="5"/>
-        <v>7.6102770935565838E-3</v>
-      </c>
-      <c r="L20">
+        <v>0.36887271402988014</v>
+      </c>
+      <c r="N20">
         <f t="shared" si="6"/>
-        <v>3.1143312331236324</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="7"/>
-        <v>0.46714968496854481</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="8"/>
-        <v>0.46714968496854481</v>
+        <v>0.2370092364518861</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.3">
@@ -2634,7 +2666,7 @@
         <v>0.16</v>
       </c>
       <c r="D21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E21">
@@ -2650,32 +2682,32 @@
         <v>0.24492363761346614</v>
       </c>
       <c r="H21">
+        <f>G21*SQRT($H$4)/$H$2</f>
+        <v>1.632824250756441</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="3"/>
-        <v>4.8984727522693223</v>
-      </c>
-      <c r="I21">
+        <v>0.26125188012103057</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K21">
+        <f>($H$3+I21/J21)*$H$2</f>
+        <v>1.0546945504538646E-2</v>
+      </c>
+      <c r="L21">
         <f t="shared" si="4"/>
-        <v>0.78375564036309164</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K21">
+        <v>2.3222234106364601</v>
+      </c>
+      <c r="M21">
         <f t="shared" si="5"/>
-        <v>8.3375564036309163E-3</v>
-      </c>
-      <c r="L21">
+        <v>0.37155574570183364</v>
+      </c>
+      <c r="N21">
         <f t="shared" si="6"/>
-        <v>2.9375949709534144</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="7"/>
-        <v>0.47001519535254632</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="8"/>
-        <v>0.47001519535254632</v>
+        <v>0.26125188012103057</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.3">
@@ -2683,7 +2715,7 @@
         <v>0.17</v>
       </c>
       <c r="D22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E22">
@@ -2699,32 +2731,32 @@
         <v>0.2524814149174115</v>
       </c>
       <c r="H22">
+        <f>G22*SQRT($H$4)/$H$2</f>
+        <v>1.6832094327827434</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="3"/>
-        <v>5.0496282983482299</v>
-      </c>
-      <c r="I22">
+        <v>0.2861456035730664</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K22">
+        <f>($H$3+I22/J22)*$H$2</f>
+        <v>1.1480460133989989E-2</v>
+      </c>
+      <c r="L22">
         <f t="shared" si="4"/>
-        <v>0.85843681071919919</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K22">
+        <v>2.19922731293578</v>
+      </c>
+      <c r="M22">
         <f t="shared" si="5"/>
-        <v>9.084368107191992E-3</v>
-      </c>
-      <c r="L22">
+        <v>0.37386864319908264</v>
+      </c>
+      <c r="N22">
         <f t="shared" si="6"/>
-        <v>2.7792952898674899</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="7"/>
-        <v>0.47248019927747331</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="8"/>
-        <v>0.47248019927747331</v>
+        <v>0.2861456035730664</v>
       </c>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.3">
@@ -2732,7 +2764,7 @@
         <v>0.18</v>
       </c>
       <c r="D23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E23">
@@ -2748,32 +2780,32 @@
         <v>0.25971023456838249</v>
       </c>
       <c r="H23">
+        <f>G23*SQRT($H$4)/$H$2</f>
+        <v>1.7314015637892168</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="3"/>
-        <v>5.1942046913676503</v>
-      </c>
-      <c r="I23">
+        <v>0.31165228148205903</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K23">
+        <f>($H$3+I23/J23)*$H$2</f>
+        <v>1.2436960555577215E-2</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="4"/>
-        <v>0.93495684444617699</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K23">
+        <v>2.0882130598373441</v>
+      </c>
+      <c r="M23">
         <f t="shared" si="5"/>
-        <v>9.8495684444617707E-3</v>
-      </c>
-      <c r="L23">
+        <v>0.3758783507707219</v>
+      </c>
+      <c r="N23">
         <f t="shared" si="6"/>
-        <v>2.6367676516265313</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="7"/>
-        <v>0.47461817729277561</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="8"/>
-        <v>0.47461817729277561</v>
+        <v>0.31165228148205903</v>
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.3">
@@ -2781,7 +2813,7 @@
         <v>0.19</v>
       </c>
       <c r="D24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E24">
@@ -2797,32 +2829,32 @@
         <v>0.26663450042597275</v>
       </c>
       <c r="H24">
+        <f>G24*SQRT($H$4)/$H$2</f>
+        <v>1.777563336173152</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="3"/>
-        <v>5.3326900085194557</v>
-      </c>
-      <c r="I24">
+        <v>0.33773703387289888</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K24">
+        <f>($H$3+I24/J24)*$H$2</f>
+        <v>1.3415138770233708E-2</v>
+      </c>
+      <c r="L24">
         <f t="shared" si="4"/>
-        <v>1.0132111016186967</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K24">
+        <v>1.9875642361419097</v>
+      </c>
+      <c r="M24">
         <f t="shared" si="5"/>
-        <v>1.0632111016186966E-2</v>
-      </c>
-      <c r="L24">
+        <v>0.37763720486696284</v>
+      </c>
+      <c r="N24">
         <f t="shared" si="6"/>
-        <v>2.507822764642246</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="7"/>
-        <v>0.47648632528202672</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="8"/>
-        <v>0.47648632528202672</v>
+        <v>0.33773703387289888</v>
       </c>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.3">
@@ -2830,7 +2862,7 @@
         <v>0.2</v>
       </c>
       <c r="D25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E25">
@@ -2846,32 +2878,32 @@
         <v>0.27327588325319851</v>
       </c>
       <c r="H25">
+        <f>G25*SQRT($H$4)/$H$2</f>
+        <v>1.8218392216879904</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="3"/>
-        <v>5.4655176650639703</v>
-      </c>
-      <c r="I25">
+        <v>0.36436784433759811</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K25">
+        <f>($H$3+I25/J25)*$H$2</f>
+        <v>1.4413794162659928E-2</v>
+      </c>
+      <c r="L25">
         <f t="shared" si="4"/>
-        <v>1.0931035330127941</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K25">
+        <v>1.8959330220015302</v>
+      </c>
+      <c r="M25">
         <f t="shared" si="5"/>
-        <v>1.1431035330127941E-2</v>
-      </c>
-      <c r="L25">
+        <v>0.37918660440030605</v>
+      </c>
+      <c r="N25">
         <f t="shared" si="6"/>
-        <v>2.3906485752252498</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="7"/>
-        <v>0.47812971504504997</v>
-      </c>
-      <c r="N25">
-        <f t="shared" si="8"/>
-        <v>0.47812971504504997</v>
+        <v>0.36436784433759811</v>
       </c>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.3">
@@ -2879,7 +2911,7 @@
         <v>0.21</v>
       </c>
       <c r="D26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E26">
@@ -2895,32 +2927,32 @@
         <v>0.27965374112567021</v>
       </c>
       <c r="H26">
+        <f>G26*SQRT($H$4)/$H$2</f>
+        <v>1.8643582741711349</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="3"/>
-        <v>5.5930748225134046</v>
-      </c>
-      <c r="I26">
+        <v>0.39151523757593831</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K26">
+        <f>($H$3+I26/J26)*$H$2</f>
+        <v>1.5431821409097685E-2</v>
+      </c>
+      <c r="L26">
         <f t="shared" si="4"/>
-        <v>1.1745457127278149</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K26">
+        <v>1.8121888124029417</v>
+      </c>
+      <c r="M26">
         <f t="shared" si="5"/>
-        <v>1.2245457127278149E-2</v>
-      </c>
-      <c r="L26">
+        <v>0.38055965060461777</v>
+      </c>
+      <c r="N26">
         <f t="shared" si="6"/>
-        <v>2.2837345982185484</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="7"/>
-        <v>0.47958426562589512</v>
-      </c>
-      <c r="N26">
-        <f t="shared" si="8"/>
-        <v>0.47958426562589512</v>
+        <v>0.38055965060461777</v>
       </c>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.3">
@@ -2928,7 +2960,7 @@
         <v>0.22</v>
       </c>
       <c r="D27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E27">
@@ -2944,32 +2976,32 @@
         <v>0.28578545772504932</v>
       </c>
       <c r="H27">
+        <f>G27*SQRT($H$4)/$H$2</f>
+        <v>1.9052363848336622</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="3"/>
-        <v>5.7157091545009866</v>
-      </c>
-      <c r="I27">
+        <v>0.41915200466340569</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K27">
+        <f>($H$3+I27/J27)*$H$2</f>
+        <v>1.6468200174877712E-2</v>
+      </c>
+      <c r="L27">
         <f t="shared" si="4"/>
-        <v>1.2574560139902171</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K27">
+        <v>1.7353776046578295</v>
+      </c>
+      <c r="M27">
         <f t="shared" si="5"/>
-        <v>1.3074560139902172E-2</v>
-      </c>
-      <c r="L27">
+        <v>0.38178307302472247</v>
+      </c>
+      <c r="N27">
         <f t="shared" si="6"/>
-        <v>2.1858131720459366</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="7"/>
-        <v>0.48087889785010607</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="8"/>
-        <v>0.48087889785010607</v>
+        <v>0.38178307302472247</v>
       </c>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.3">
@@ -2977,48 +3009,48 @@
         <v>0.23</v>
       </c>
       <c r="D28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E28">
-        <f t="shared" ref="E28:E43" si="11">D28*C28</f>
+        <f t="shared" ref="E28:E43" si="9">D28*C28</f>
         <v>0.23</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F28:F43" si="12">D28+2*C28</f>
+        <f t="shared" ref="F28:F43" si="10">D28+2*C28</f>
         <v>1.46</v>
       </c>
       <c r="G28">
-        <f t="shared" ref="G28:G43" si="13">(E28/F28)^(2/3)</f>
+        <f t="shared" ref="G28:G43" si="11">(E28/F28)^(2/3)</f>
         <v>0.29168671772025279</v>
       </c>
       <c r="H28">
-        <f t="shared" si="3"/>
-        <v>5.8337343544050562</v>
+        <f>G28*SQRT($H$4)/$H$2</f>
+        <v>1.9445781181350188</v>
       </c>
       <c r="I28">
-        <f t="shared" ref="I28:I43" si="14">H28*E28</f>
-        <v>1.341758901513163</v>
+        <f t="shared" ref="I28:I43" si="12">H28*E28</f>
+        <v>0.44725296717105434</v>
       </c>
       <c r="J28">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
+        <f t="shared" si="8"/>
+        <v>0.4</v>
       </c>
       <c r="K28">
-        <f t="shared" si="5"/>
-        <v>1.3917589015131631E-2</v>
+        <f>($H$3+I28/J28)*$H$2</f>
+        <v>1.7521986268914536E-2</v>
       </c>
       <c r="L28">
-        <f t="shared" ref="L28:L43" si="15">G28*SQRT($H$4)/K28</f>
-        <v>2.0958135593968326</v>
+        <f t="shared" ref="L28:L43" si="13">G28*SQRT($H$4)/K28</f>
+        <v>1.664689797398879</v>
       </c>
       <c r="M28">
-        <f t="shared" ref="M28:M43" si="16">L28*E28</f>
-        <v>0.48203711866127152</v>
+        <f t="shared" ref="M28:M43" si="14">L28*E28</f>
+        <v>0.38287865340174221</v>
       </c>
       <c r="N28">
-        <f t="shared" si="8"/>
-        <v>0.48203711866127152</v>
+        <f t="shared" si="6"/>
+        <v>0.38287865340174221</v>
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.3">
@@ -3026,48 +3058,48 @@
         <v>0.24</v>
       </c>
       <c r="D29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E29">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E29">
+        <v>0.24</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="10"/>
+        <v>1.48</v>
+      </c>
+      <c r="G29">
         <f t="shared" si="11"/>
-        <v>0.24</v>
-      </c>
-      <c r="F29">
+        <v>0.29737173327869948</v>
+      </c>
+      <c r="H29">
+        <f>G29*SQRT($H$4)/$H$2</f>
+        <v>1.9824782218579966</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="12"/>
-        <v>1.48</v>
-      </c>
-      <c r="G29">
+        <v>0.47579477324591918</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K29">
+        <f>($H$3+I29/J29)*$H$2</f>
+        <v>1.859230399672197E-2</v>
+      </c>
+      <c r="L29">
         <f t="shared" si="13"/>
-        <v>0.29737173327869948</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="3"/>
-        <v>5.94743466557399</v>
-      </c>
-      <c r="I29">
+        <v>1.5994345473865392</v>
+      </c>
+      <c r="M29">
         <f t="shared" si="14"/>
-        <v>1.4273843197377576</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="5"/>
-        <v>1.4773843197377576E-2</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="15"/>
-        <v>2.0128258389224296</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="16"/>
-        <v>0.48307820134138307</v>
+        <v>0.3838642913727694</v>
       </c>
       <c r="N29">
-        <f t="shared" si="8"/>
-        <v>0.48307820134138307</v>
+        <f t="shared" si="6"/>
+        <v>0.3838642913727694</v>
       </c>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.3">
@@ -3075,48 +3107,48 @@
         <v>0.25</v>
       </c>
       <c r="D30">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E30">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E30">
+        <v>0.25</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="10"/>
+        <v>1.5</v>
+      </c>
+      <c r="G30">
         <f t="shared" si="11"/>
-        <v>0.25</v>
-      </c>
-      <c r="F30">
+        <v>0.30285343213868998</v>
+      </c>
+      <c r="H30">
+        <f>G30*SQRT($H$4)/$H$2</f>
+        <v>2.0190228809246</v>
+      </c>
+      <c r="I30">
         <f t="shared" si="12"/>
-        <v>1.5</v>
-      </c>
-      <c r="G30">
+        <v>0.50475572023115001</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K30">
+        <f>($H$3+I30/J30)*$H$2</f>
+        <v>1.9678339508668121E-2</v>
+      </c>
+      <c r="L30">
         <f t="shared" si="13"/>
-        <v>0.30285343213868998</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="3"/>
-        <v>6.0570686427737996</v>
-      </c>
-      <c r="I30">
+        <v>1.5390192450195603</v>
+      </c>
+      <c r="M30">
         <f t="shared" si="14"/>
-        <v>1.5142671606934499</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="5"/>
-        <v>1.56426716069345E-2</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="15"/>
-        <v>1.9360723011306653</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="16"/>
-        <v>0.48401807528266633</v>
+        <v>0.38475481125489008</v>
       </c>
       <c r="N30">
-        <f t="shared" si="8"/>
-        <v>0.48401807528266633</v>
+        <f t="shared" si="6"/>
+        <v>0.38475481125489008</v>
       </c>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.3">
@@ -3124,48 +3156,48 @@
         <v>0.26</v>
       </c>
       <c r="D31">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E31">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E31">
+        <v>0.26</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="10"/>
+        <v>1.52</v>
+      </c>
+      <c r="G31">
         <f t="shared" si="11"/>
-        <v>0.26</v>
-      </c>
-      <c r="F31">
+        <v>0.3081436151028345</v>
+      </c>
+      <c r="H31">
+        <f>G31*SQRT($H$4)/$H$2</f>
+        <v>2.0542907673522302</v>
+      </c>
+      <c r="I31">
         <f t="shared" si="12"/>
-        <v>1.52</v>
-      </c>
-      <c r="G31">
+        <v>0.53411559951157983</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K31">
+        <f>($H$3+I31/J31)*$H$2</f>
+        <v>2.0779334981684244E-2</v>
+      </c>
+      <c r="L31">
         <f t="shared" si="13"/>
-        <v>0.3081436151028345</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="3"/>
-        <v>6.16287230205669</v>
-      </c>
-      <c r="I31">
+        <v>1.4829329974921956</v>
+      </c>
+      <c r="M31">
         <f t="shared" si="14"/>
-        <v>1.6023467985347395</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="5"/>
-        <v>1.6523467985347394E-2</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="15"/>
-        <v>1.8648846318223797</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="16"/>
-        <v>0.48487000427381877</v>
+        <v>0.38556257934797089</v>
       </c>
       <c r="N31">
-        <f t="shared" si="8"/>
-        <v>0.48487000427381877</v>
+        <f t="shared" si="6"/>
+        <v>0.38556257934797089</v>
       </c>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.3">
@@ -3173,48 +3205,48 @@
         <v>0.27</v>
       </c>
       <c r="D32">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E32">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E32">
+        <v>0.27</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="10"/>
+        <v>1.54</v>
+      </c>
+      <c r="G32">
         <f t="shared" si="11"/>
-        <v>0.27</v>
-      </c>
-      <c r="F32">
+        <v>0.31325308895252124</v>
+      </c>
+      <c r="H32">
+        <f>G32*SQRT($H$4)/$H$2</f>
+        <v>2.0883539263501416</v>
+      </c>
+      <c r="I32">
         <f t="shared" si="12"/>
-        <v>1.54</v>
-      </c>
-      <c r="G32">
+        <v>0.5638555601145383</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K32">
+        <f>($H$3+I32/J32)*$H$2</f>
+        <v>2.1894583504295184E-2</v>
+      </c>
+      <c r="L32">
         <f t="shared" si="13"/>
-        <v>0.31325308895252124</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="3"/>
-        <v>6.2650617790504253</v>
-      </c>
-      <c r="I32">
+        <v>1.4307332628230567</v>
+      </c>
+      <c r="M32">
         <f t="shared" si="14"/>
-        <v>1.6915666803436149</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="5"/>
-        <v>1.7415666803436151E-2</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="15"/>
-        <v>1.7986855886029911</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="16"/>
-        <v>0.48564510892280766</v>
+        <v>0.38629798096222534</v>
       </c>
       <c r="N32">
-        <f t="shared" si="8"/>
-        <v>0.48564510892280766</v>
+        <f t="shared" si="6"/>
+        <v>0.38629798096222534</v>
       </c>
     </row>
     <row r="33" spans="3:14" x14ac:dyDescent="0.3">
@@ -3222,48 +3254,48 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="D33">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E33">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E33">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="10"/>
+        <v>1.56</v>
+      </c>
+      <c r="G33">
         <f t="shared" si="11"/>
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="F33">
+        <v>0.31819177941838417</v>
+      </c>
+      <c r="H33">
+        <f>G33*SQRT($H$4)/$H$2</f>
+        <v>2.1212785294558945</v>
+      </c>
+      <c r="I33">
         <f t="shared" si="12"/>
-        <v>1.56</v>
-      </c>
-      <c r="G33">
+        <v>0.59395798824765056</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K33">
+        <f>($H$3+I33/J33)*$H$2</f>
+        <v>2.3023424559286895E-2</v>
+      </c>
+      <c r="L33">
         <f t="shared" si="13"/>
-        <v>0.31819177941838417</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="3"/>
-        <v>6.3638355883676834</v>
-      </c>
-      <c r="I33">
+        <v>1.3820349731162649</v>
+      </c>
+      <c r="M33">
         <f t="shared" si="14"/>
-        <v>1.7818739647429516</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="5"/>
-        <v>1.8318739647429517E-2</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="15"/>
-        <v>1.7369741889586428</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="16"/>
-        <v>0.48635277290841999</v>
+        <v>0.3869697924725542</v>
       </c>
       <c r="N33">
-        <f t="shared" si="8"/>
-        <v>0.48635277290841999</v>
+        <f t="shared" si="6"/>
+        <v>0.3869697924725542</v>
       </c>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.3">
@@ -3271,48 +3303,48 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="D34">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E34">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E34">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="10"/>
+        <v>1.58</v>
+      </c>
+      <c r="G34">
         <f t="shared" si="11"/>
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="F34">
+        <v>0.32296882782654257</v>
+      </c>
+      <c r="H34">
+        <f>G34*SQRT($H$4)/$H$2</f>
+        <v>2.1531255188436176</v>
+      </c>
+      <c r="I34">
         <f t="shared" si="12"/>
-        <v>1.58</v>
-      </c>
-      <c r="G34">
+        <v>0.62440640046464901</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K34">
+        <f>($H$3+I34/J34)*$H$2</f>
+        <v>2.4165240017424337E-2</v>
+      </c>
+      <c r="L34">
         <f t="shared" si="13"/>
-        <v>0.32296882782654257</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="3"/>
-        <v>6.4593765565308514</v>
-      </c>
-      <c r="I34">
+        <v>1.336501634553044</v>
+      </c>
+      <c r="M34">
         <f t="shared" si="14"/>
-        <v>1.8732192013939468</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="5"/>
-        <v>1.923219201393947E-2</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="15"/>
-        <v>1.6793136611388613</v>
-      </c>
-      <c r="M34">
-        <f t="shared" si="16"/>
-        <v>0.48700096173026974</v>
+        <v>0.38758547402038274</v>
       </c>
       <c r="N34">
-        <f t="shared" si="8"/>
-        <v>0.48700096173026974</v>
+        <f t="shared" si="6"/>
+        <v>0.38758547402038274</v>
       </c>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.3">
@@ -3320,48 +3352,48 @@
         <v>0.3</v>
       </c>
       <c r="D35">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E35">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E35">
+        <v>0.3</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="10"/>
+        <v>1.6</v>
+      </c>
+      <c r="G35">
         <f t="shared" si="11"/>
-        <v>0.3</v>
-      </c>
-      <c r="F35">
+        <v>0.32759267427611211</v>
+      </c>
+      <c r="H35">
+        <f>G35*SQRT($H$4)/$H$2</f>
+        <v>2.1839511618407474</v>
+      </c>
+      <c r="I35">
         <f t="shared" si="12"/>
-        <v>1.6</v>
-      </c>
-      <c r="G35">
+        <v>0.65518534855222421</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K35">
+        <f>($H$3+I35/J35)*$H$2</f>
+        <v>2.5319450570708404E-2</v>
+      </c>
+      <c r="L35">
         <f t="shared" si="13"/>
-        <v>0.32759267427611211</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="3"/>
-        <v>6.5518534855222423</v>
-      </c>
-      <c r="I35">
+        <v>1.2938380055335716</v>
+      </c>
+      <c r="M35">
         <f t="shared" si="14"/>
-        <v>1.9655560456566725</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K35">
-        <f t="shared" si="5"/>
-        <v>2.0155560456566725E-2</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="15"/>
-        <v>1.6253215830045635</v>
-      </c>
-      <c r="M35">
-        <f t="shared" si="16"/>
-        <v>0.48759647490136904</v>
+        <v>0.3881514016600715</v>
       </c>
       <c r="N35">
-        <f t="shared" si="8"/>
-        <v>0.48759647490136904</v>
+        <f t="shared" si="6"/>
+        <v>0.3881514016600715</v>
       </c>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.3">
@@ -3369,48 +3401,48 @@
         <v>0.31</v>
       </c>
       <c r="D36">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E36">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E36">
+        <v>0.31</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="10"/>
+        <v>1.62</v>
+      </c>
+      <c r="G36">
         <f t="shared" si="11"/>
-        <v>0.31</v>
-      </c>
-      <c r="F36">
+        <v>0.33207112962159829</v>
+      </c>
+      <c r="H36">
+        <f>G36*SQRT($H$4)/$H$2</f>
+        <v>2.2138075308106551</v>
+      </c>
+      <c r="I36">
         <f t="shared" si="12"/>
-        <v>1.62</v>
-      </c>
-      <c r="G36">
+        <v>0.68628033455130311</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K36">
+        <f>($H$3+I36/J36)*$H$2</f>
+        <v>2.6485512545673866E-2</v>
+      </c>
+      <c r="L36">
         <f t="shared" si="13"/>
-        <v>0.33207112962159829</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="3"/>
-        <v>6.6414225924319652</v>
-      </c>
-      <c r="I36">
+        <v>1.253784041554592</v>
+      </c>
+      <c r="M36">
         <f t="shared" si="14"/>
-        <v>2.0588410036539093</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K36">
-        <f t="shared" si="5"/>
-        <v>2.1088410036539093E-2</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="15"/>
-        <v>1.5746617646670904</v>
-      </c>
-      <c r="M36">
-        <f t="shared" si="16"/>
-        <v>0.48814514704679801</v>
+        <v>0.3886730528819235</v>
       </c>
       <c r="N36">
-        <f t="shared" si="8"/>
-        <v>0.48814514704679801</v>
+        <f t="shared" si="6"/>
+        <v>0.3886730528819235</v>
       </c>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.3">
@@ -3418,48 +3450,48 @@
         <v>0.32</v>
       </c>
       <c r="D37">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E37">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E37">
+        <v>0.32</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="10"/>
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="G37">
         <f t="shared" si="11"/>
-        <v>0.32</v>
-      </c>
-      <c r="F37">
+        <v>0.33641143808612001</v>
+      </c>
+      <c r="H37">
+        <f>G37*SQRT($H$4)/$H$2</f>
+        <v>2.2427429205741336</v>
+      </c>
+      <c r="I37">
         <f t="shared" si="12"/>
-        <v>1.6400000000000001</v>
-      </c>
-      <c r="G37">
+        <v>0.71767773458372275</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K37">
+        <f>($H$3+I37/J37)*$H$2</f>
+        <v>2.76629150468896E-2</v>
+      </c>
+      <c r="L37">
         <f t="shared" si="13"/>
-        <v>0.33641143808612001</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="3"/>
-        <v>6.7282287617224004</v>
-      </c>
-      <c r="I37">
+        <v>1.216109862304428</v>
+      </c>
+      <c r="M37">
         <f t="shared" si="14"/>
-        <v>2.1530332037511681</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K37">
-        <f t="shared" si="5"/>
-        <v>2.2030332037511681E-2</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="15"/>
-        <v>1.5270375294993401</v>
-      </c>
-      <c r="M37">
-        <f t="shared" si="16"/>
-        <v>0.48865200943978887</v>
+        <v>0.38915515593741695</v>
       </c>
       <c r="N37">
-        <f t="shared" si="8"/>
-        <v>0.48865200943978887</v>
+        <f t="shared" si="6"/>
+        <v>0.38915515593741695</v>
       </c>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.3">
@@ -3467,48 +3499,48 @@
         <v>0.33</v>
       </c>
       <c r="D38">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E38">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E38">
+        <v>0.33</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="10"/>
+        <v>1.6600000000000001</v>
+      </c>
+      <c r="G38">
         <f t="shared" si="11"/>
-        <v>0.33</v>
-      </c>
-      <c r="F38">
+        <v>0.34062033198365266</v>
+      </c>
+      <c r="H38">
+        <f>G38*SQRT($H$4)/$H$2</f>
+        <v>2.2708022132243513</v>
+      </c>
+      <c r="I38">
         <f t="shared" si="12"/>
-        <v>1.6600000000000001</v>
-      </c>
-      <c r="G38">
+        <v>0.74936473036403595</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K38">
+        <f>($H$3+I38/J38)*$H$2</f>
+        <v>2.8851177388651346E-2</v>
+      </c>
+      <c r="L38">
         <f t="shared" si="13"/>
-        <v>0.34062033198365266</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="3"/>
-        <v>6.8124066396730534</v>
-      </c>
-      <c r="I38">
+        <v>1.1806115479974699</v>
+      </c>
+      <c r="M38">
         <f t="shared" si="14"/>
-        <v>2.2480941910921075</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="5"/>
-        <v>2.2980941910921072E-2</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="15"/>
-        <v>1.4821861231970743</v>
-      </c>
-      <c r="M38">
-        <f t="shared" si="16"/>
-        <v>0.48912142065503456</v>
+        <v>0.38960181083916512</v>
       </c>
       <c r="N38">
-        <f t="shared" si="8"/>
-        <v>0.48912142065503456</v>
+        <f t="shared" si="6"/>
+        <v>0.38960181083916512</v>
       </c>
     </row>
     <row r="39" spans="3:14" x14ac:dyDescent="0.3">
@@ -3516,48 +3548,48 @@
         <v>0.34</v>
       </c>
       <c r="D39">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E39">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E39">
+        <v>0.34</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="10"/>
+        <v>1.6800000000000002</v>
+      </c>
+      <c r="G39">
         <f t="shared" si="11"/>
-        <v>0.34</v>
-      </c>
-      <c r="F39">
+        <v>0.34470407975589484</v>
+      </c>
+      <c r="H39">
+        <f>G39*SQRT($H$4)/$H$2</f>
+        <v>2.2980271983726324</v>
+      </c>
+      <c r="I39">
         <f t="shared" si="12"/>
-        <v>1.6800000000000002</v>
-      </c>
-      <c r="G39">
+        <v>0.78132924744669507</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K39">
+        <f>($H$3+I39/J39)*$H$2</f>
+        <v>3.0049846779251065E-2</v>
+      </c>
+      <c r="L39">
         <f t="shared" si="13"/>
-        <v>0.34470407975589484</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="3"/>
-        <v>6.8940815951178971</v>
-      </c>
-      <c r="I39">
+        <v>1.1471076118561359</v>
+      </c>
+      <c r="M39">
         <f t="shared" si="14"/>
-        <v>2.3439877423400852</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K39">
-        <f t="shared" si="5"/>
-        <v>2.3939877423400851E-2</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="15"/>
-        <v>1.4398740380305877</v>
-      </c>
-      <c r="M39">
-        <f t="shared" si="16"/>
-        <v>0.48955717293039985</v>
+        <v>0.39001658803108624</v>
       </c>
       <c r="N39">
-        <f t="shared" si="8"/>
-        <v>0.48955717293039985</v>
+        <f t="shared" si="6"/>
+        <v>0.39001658803108624</v>
       </c>
     </row>
     <row r="40" spans="3:14" x14ac:dyDescent="0.3">
@@ -3565,48 +3597,48 @@
         <v>0.35</v>
       </c>
       <c r="D40">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E40">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E40">
+        <v>0.35</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="10"/>
+        <v>1.7</v>
+      </c>
+      <c r="G40">
         <f t="shared" si="11"/>
-        <v>0.35</v>
-      </c>
-      <c r="F40">
+        <v>0.34866852831389705</v>
+      </c>
+      <c r="H40">
+        <f>G40*SQRT($H$4)/$H$2</f>
+        <v>2.3244568554259804</v>
+      </c>
+      <c r="I40">
         <f t="shared" si="12"/>
-        <v>1.7</v>
-      </c>
-      <c r="G40">
+        <v>0.81355989939909312</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K40">
+        <f>($H$3+I40/J40)*$H$2</f>
+        <v>3.1258496227465987E-2</v>
+      </c>
+      <c r="L40">
         <f t="shared" si="13"/>
-        <v>0.34866852831389705</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="3"/>
-        <v>6.9733705662779411</v>
-      </c>
-      <c r="I40">
+        <v>1.1154360266618697</v>
+      </c>
+      <c r="M40">
         <f t="shared" si="14"/>
-        <v>2.4406796981972794</v>
-      </c>
-      <c r="J40">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K40">
-        <f t="shared" si="5"/>
-        <v>2.4906796981972793E-2</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="15"/>
-        <v>1.3998930836681194</v>
-      </c>
-      <c r="M40">
-        <f t="shared" si="16"/>
-        <v>0.48996257928384174</v>
+        <v>0.39040260933165438</v>
       </c>
       <c r="N40">
-        <f t="shared" si="8"/>
-        <v>0.48996257928384174</v>
+        <f t="shared" si="6"/>
+        <v>0.39040260933165438</v>
       </c>
     </row>
     <row r="41" spans="3:14" x14ac:dyDescent="0.3">
@@ -3614,48 +3646,48 @@
         <v>0.36</v>
       </c>
       <c r="D41">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E41">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E41">
+        <v>0.36</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="10"/>
+        <v>1.72</v>
+      </c>
+      <c r="G41">
         <f t="shared" si="11"/>
-        <v>0.36</v>
-      </c>
-      <c r="F41">
+        <v>0.35251914050292288</v>
+      </c>
+      <c r="H41">
+        <f>G41*SQRT($H$4)/$H$2</f>
+        <v>2.3501276033528193</v>
+      </c>
+      <c r="I41">
         <f t="shared" si="12"/>
-        <v>1.72</v>
-      </c>
-      <c r="G41">
+        <v>0.84604593720701493</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K41">
+        <f>($H$3+I41/J41)*$H$2</f>
+        <v>3.2476722645263058E-2</v>
+      </c>
+      <c r="L41">
         <f t="shared" si="13"/>
-        <v>0.35251914050292288</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="3"/>
-        <v>7.0503828100584576</v>
-      </c>
-      <c r="I41">
+        <v>1.0854517075304089</v>
+      </c>
+      <c r="M41">
         <f t="shared" si="14"/>
-        <v>2.5381378116210445</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K41">
-        <f t="shared" si="5"/>
-        <v>2.5881378116210444E-2</v>
-      </c>
-      <c r="L41">
-        <f t="shared" si="15"/>
-        <v>1.3620570702227304</v>
-      </c>
-      <c r="M41">
-        <f t="shared" si="16"/>
-        <v>0.49034054528018289</v>
+        <v>0.3907626147109472</v>
       </c>
       <c r="N41">
-        <f t="shared" si="8"/>
-        <v>0.49034054528018289</v>
+        <f t="shared" si="6"/>
+        <v>0.3907626147109472</v>
       </c>
     </row>
     <row r="42" spans="3:14" x14ac:dyDescent="0.3">
@@ -3663,48 +3695,48 @@
         <v>0.37</v>
       </c>
       <c r="D42">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E42">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E42">
+        <v>0.37</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="10"/>
+        <v>1.74</v>
+      </c>
+      <c r="G42">
         <f t="shared" si="11"/>
-        <v>0.37</v>
-      </c>
-      <c r="F42">
+        <v>0.35626102837124329</v>
+      </c>
+      <c r="H42">
+        <f>G42*SQRT($H$4)/$H$2</f>
+        <v>2.3750735224749553</v>
+      </c>
+      <c r="I42">
         <f t="shared" si="12"/>
-        <v>1.74</v>
-      </c>
-      <c r="G42">
+        <v>0.8787772033157335</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K42">
+        <f>($H$3+I42/J42)*$H$2</f>
+        <v>3.3704145124340001E-2</v>
+      </c>
+      <c r="L42">
         <f t="shared" si="13"/>
-        <v>0.35626102837124329</v>
-      </c>
-      <c r="H42">
-        <f t="shared" si="3"/>
-        <v>7.1252205674248659</v>
-      </c>
-      <c r="I42">
+        <v>1.0570243720970793</v>
+      </c>
+      <c r="M42">
         <f t="shared" si="14"/>
-        <v>2.6363316099472005</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K42">
-        <f t="shared" si="5"/>
-        <v>2.6863316099472005E-2</v>
-      </c>
-      <c r="L42">
-        <f t="shared" si="15"/>
-        <v>1.3261989958799076</v>
-      </c>
-      <c r="M42">
-        <f t="shared" si="16"/>
-        <v>0.4906936284755658</v>
+        <v>0.39109901767591937</v>
       </c>
       <c r="N42">
-        <f t="shared" si="8"/>
-        <v>0.4906936284755658</v>
+        <f t="shared" si="6"/>
+        <v>0.39109901767591937</v>
       </c>
     </row>
     <row r="43" spans="3:14" x14ac:dyDescent="0.3">
@@ -3712,48 +3744,48 @@
         <v>0.38</v>
       </c>
       <c r="D43">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E43">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E43">
+        <v>0.38</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="10"/>
+        <v>1.76</v>
+      </c>
+      <c r="G43">
         <f t="shared" si="11"/>
-        <v>0.38</v>
-      </c>
-      <c r="F43">
+        <v>0.35989898281221949</v>
+      </c>
+      <c r="H43">
+        <f>G43*SQRT($H$4)/$H$2</f>
+        <v>2.3993265520814631</v>
+      </c>
+      <c r="I43">
         <f t="shared" si="12"/>
-        <v>1.76</v>
-      </c>
-      <c r="G43">
+        <v>0.911744089790956</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="K43">
+        <f>($H$3+I43/J43)*$H$2</f>
+        <v>3.4940403367160845E-2</v>
+      </c>
+      <c r="L43">
         <f t="shared" si="13"/>
-        <v>0.35989898281221949</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="3"/>
-        <v>7.1979796562443896</v>
-      </c>
-      <c r="I43">
+        <v>1.030036714317027</v>
+      </c>
+      <c r="M43">
         <f t="shared" si="14"/>
-        <v>2.7352322693728679</v>
-      </c>
-      <c r="J43">
-        <f t="shared" si="10"/>
-        <v>0.5</v>
-      </c>
-      <c r="K43">
-        <f t="shared" si="5"/>
-        <v>2.7852322693728677E-2</v>
-      </c>
-      <c r="L43">
-        <f t="shared" si="15"/>
-        <v>1.2921686523948523</v>
-      </c>
-      <c r="M43">
-        <f t="shared" si="16"/>
-        <v>0.49102408791004387</v>
+        <v>0.39141395144047025</v>
       </c>
       <c r="N43">
-        <f t="shared" si="8"/>
-        <v>0.49102408791004387</v>
+        <f t="shared" si="6"/>
+        <v>0.39141395144047025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>